<commit_message>
Explained Everthing by Comments
</commit_message>
<xml_diff>
--- a/ExcelData/HospitalsList.xlsx
+++ b/ExcelData/HospitalsList.xlsx
@@ -68,9 +68,6 @@
     <t>Brains Super Speciality Hospital</t>
   </si>
   <si>
-    <t>Pathway Hospitals</t>
-  </si>
-  <si>
     <t>Sai Thunga Hospitals</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>SRV Agadi Hospital</t>
+  </si>
+  <si>
+    <t>Apollo Hospitals</t>
   </si>
 </sst>
 </file>
@@ -252,12 +252,12 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25">

</xml_diff>